<commit_message>
small bug fixed on student controller
</commit_message>
<xml_diff>
--- a/db-backup/import_student_sample_file(demo).xlsx
+++ b/db-backup/import_student_sample_file(demo).xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Lochan</t>
   </si>
@@ -113,6 +113,36 @@
   </si>
   <si>
     <t>Eddie</t>
+  </si>
+  <si>
+    <t>Admission Number</t>
+  </si>
+  <si>
+    <t>Symbol Number/Roll Number</t>
+  </si>
+  <si>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>Date Of Birth(BS)</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Mobile No</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Admission Date</t>
+  </si>
+  <si>
+    <t>Blood Group (O+, A+, B+, AB+, O-, A-, B-, AB-)</t>
+  </si>
+  <si>
+    <t>Gender(Male/Female)</t>
   </si>
 </sst>
 </file>
@@ -951,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -972,48 +1002,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3">
-        <v>58589</v>
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>980000000</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1">
-        <v>58589</v>
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
         <v>58589</v>
       </c>
       <c r="E2" t="s">
@@ -1022,19 +1052,28 @@
       <c r="F2">
         <v>980000000</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="H2" s="1">
-        <v>58590</v>
+        <v>58589</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
         <v>58589</v>
@@ -1046,21 +1085,21 @@
         <v>980000000</v>
       </c>
       <c r="H3" s="1">
-        <v>58591</v>
+        <v>58590</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1">
-        <v>58590</v>
+        <v>58589</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -1069,21 +1108,21 @@
         <v>980000000</v>
       </c>
       <c r="H4" s="1">
-        <v>58592</v>
+        <v>58591</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1">
-        <v>58591</v>
+        <v>58590</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -1092,21 +1131,21 @@
         <v>980000000</v>
       </c>
       <c r="H5" s="1">
-        <v>58593</v>
+        <v>58592</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1">
-        <v>58592</v>
+        <v>58591</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
@@ -1115,21 +1154,21 @@
         <v>980000000</v>
       </c>
       <c r="H6" s="1">
-        <v>58594</v>
+        <v>58593</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1">
-        <v>58593</v>
+        <v>58592</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -1138,21 +1177,21 @@
         <v>980000000</v>
       </c>
       <c r="H7" s="1">
-        <v>58595</v>
+        <v>58594</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1">
-        <v>58594</v>
+        <v>58593</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
@@ -1161,21 +1200,21 @@
         <v>980000000</v>
       </c>
       <c r="H8" s="1">
-        <v>58596</v>
+        <v>58595</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
-        <v>58595</v>
+        <v>58594</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -1184,21 +1223,21 @@
         <v>980000000</v>
       </c>
       <c r="H9" s="1">
-        <v>58597</v>
+        <v>58596</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1">
-        <v>58596</v>
+        <v>58595</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
@@ -1207,21 +1246,21 @@
         <v>980000000</v>
       </c>
       <c r="H10" s="1">
-        <v>58598</v>
+        <v>58597</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1">
-        <v>58597</v>
+        <v>58596</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
@@ -1230,21 +1269,21 @@
         <v>980000000</v>
       </c>
       <c r="H11" s="1">
-        <v>58599</v>
+        <v>58598</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1">
-        <v>58598</v>
+        <v>58597</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
@@ -1253,372 +1292,395 @@
         <v>980000000</v>
       </c>
       <c r="H12" s="1">
-        <v>58600</v>
+        <v>58599</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="1">
-        <v>58599</v>
+        <v>58598</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
       </c>
       <c r="F13">
         <v>980000000</v>
       </c>
       <c r="H13" s="1">
-        <v>58601</v>
+        <v>58600</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1">
-        <v>58600</v>
+        <v>58599</v>
       </c>
       <c r="F14">
         <v>980000000</v>
       </c>
       <c r="H14" s="1">
-        <v>58602</v>
+        <v>58601</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1">
-        <v>58601</v>
+        <v>58600</v>
       </c>
       <c r="F15">
         <v>980000000</v>
       </c>
       <c r="H15" s="1">
-        <v>58603</v>
+        <v>58602</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1">
-        <v>58602</v>
+        <v>58601</v>
       </c>
       <c r="F16">
         <v>980000000</v>
       </c>
       <c r="H16" s="1">
-        <v>58604</v>
+        <v>58603</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1">
-        <v>58603</v>
+        <v>58602</v>
       </c>
       <c r="F17">
         <v>980000000</v>
       </c>
       <c r="H17" s="1">
-        <v>58605</v>
+        <v>58604</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1">
-        <v>58604</v>
+        <v>58603</v>
       </c>
       <c r="F18">
         <v>980000000</v>
       </c>
       <c r="H18" s="1">
-        <v>58606</v>
+        <v>58605</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1">
-        <v>58605</v>
+        <v>58604</v>
       </c>
       <c r="F19">
         <v>980000000</v>
       </c>
       <c r="H19" s="1">
-        <v>58607</v>
+        <v>58606</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1">
-        <v>58606</v>
+        <v>58605</v>
       </c>
       <c r="F20">
         <v>980000000</v>
       </c>
       <c r="H20" s="1">
-        <v>58608</v>
+        <v>58607</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="1">
-        <v>58607</v>
+        <v>58606</v>
       </c>
       <c r="F21">
         <v>980000000</v>
       </c>
       <c r="H21" s="1">
-        <v>58609</v>
+        <v>58608</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="1">
-        <v>58608</v>
+        <v>58607</v>
       </c>
       <c r="F22">
         <v>980000000</v>
       </c>
       <c r="H22" s="1">
-        <v>58610</v>
+        <v>58609</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1">
-        <v>58609</v>
+        <v>58608</v>
       </c>
       <c r="F23">
         <v>980000000</v>
       </c>
       <c r="H23" s="1">
-        <v>58611</v>
+        <v>58610</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="1">
-        <v>58610</v>
+        <v>58609</v>
       </c>
       <c r="F24">
         <v>980000000</v>
       </c>
       <c r="H24" s="1">
-        <v>58612</v>
+        <v>58611</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="1">
-        <v>58611</v>
+        <v>58610</v>
       </c>
       <c r="F25">
         <v>980000000</v>
       </c>
       <c r="H25" s="1">
-        <v>58613</v>
+        <v>58612</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1">
-        <v>58612</v>
+        <v>58611</v>
       </c>
       <c r="F26">
         <v>980000000</v>
       </c>
       <c r="H26" s="1">
-        <v>58614</v>
+        <v>58613</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D27" s="1">
-        <v>58613</v>
+        <v>58612</v>
       </c>
       <c r="F27">
         <v>980000000</v>
       </c>
       <c r="H27" s="1">
-        <v>58615</v>
+        <v>58614</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D28" s="1">
-        <v>58614</v>
+        <v>58613</v>
       </c>
       <c r="F28">
         <v>980000000</v>
       </c>
       <c r="H28" s="1">
-        <v>58616</v>
+        <v>58615</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="1">
-        <v>58615</v>
+        <v>58614</v>
       </c>
       <c r="F29">
         <v>980000000</v>
       </c>
       <c r="H29" s="1">
-        <v>58617</v>
+        <v>58616</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="1">
+        <v>58615</v>
+      </c>
+      <c r="F30">
+        <v>980000000</v>
+      </c>
+      <c r="H30" s="1">
+        <v>58617</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>30</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D31" s="1">
         <v>58616</v>
       </c>
-      <c r="F30">
-        <v>980000000</v>
-      </c>
-      <c r="H30" s="1">
+      <c r="F31">
+        <v>980000000</v>
+      </c>
+      <c r="H31" s="1">
         <v>58618</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G1" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>